<commit_message>
Updated with program output.
</commit_message>
<xml_diff>
--- a/hw2/hw2/output.xlsx
+++ b/hw2/hw2/output.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mudit Vats\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\cse674\hw2\hw2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4999661E-F9DE-4099-A698-CC7463561A62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33E971E-2CBB-45F0-81B9-5459F862F3D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="1380" windowWidth="21615" windowHeight="11385" xr2:uid="{0773D6EB-A131-4237-A2C7-D65C767F5663}"/>
+    <workbookView xWindow="2070" yWindow="885" windowWidth="26475" windowHeight="13335" xr2:uid="{0773D6EB-A131-4237-A2C7-D65C767F5663}"/>
   </bookViews>
   <sheets>
     <sheet name="Ascending" sheetId="1" r:id="rId1"/>
     <sheet name="Descending" sheetId="2" r:id="rId2"/>
     <sheet name="Random" sheetId="3" r:id="rId3"/>
+    <sheet name="Program Output" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="272">
   <si>
     <t>Bubble w/Flag</t>
   </si>
@@ -65,6 +66,794 @@
   </si>
   <si>
     <t>See tabs below for Asceding, Descending and Random.</t>
+  </si>
+  <si>
+    <t>In the chart to the right we see the Time (vertical axis) vs Step (horizontal axis). 
+We can make the observation that Bubble, Bubble w/Flag, Insertion and Selection sort growth is significantly higher then the other sorting methods.
+The data also suggests that Counting Sort, followed by Quick Sort, perform the best on unorderd randomized data as the number of steps increase.</t>
+  </si>
+  <si>
+    <t>In the chart to the right we see the Time (vertical axis) vs Step (horizontal axis). 
+We can make the observation that Bubble and Selection sort growth is significantly higher then the other sorting methods.
+Bubble w/Flag and Insertion perform very well when the data is already sorted.
+The data also suggests that Counting Sort, followed by Quick Sort and Smooth Sort, perform the best on unorderd randomized data as the number of steps increase.</t>
+  </si>
+  <si>
+    <t>============================================</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ascending</t>
+  </si>
+  <si>
+    <t>BubbleSort 1000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>BubbleSort 2000 1 1 1 1</t>
+  </si>
+  <si>
+    <t>BubbleSort 4000 4 4 4 4</t>
+  </si>
+  <si>
+    <t>BubbleSort 8000 20 17 17 18</t>
+  </si>
+  <si>
+    <t>BubbleSort 16000 69 70 69 69</t>
+  </si>
+  <si>
+    <t>BubbleSort 32000 283 283 290 285</t>
+  </si>
+  <si>
+    <t>BubbleSort 64000 1136 1137 1128 1133</t>
+  </si>
+  <si>
+    <t>BubbleSort 128000 4527 4544 4539 4536</t>
+  </si>
+  <si>
+    <t>BubbleSort 256000 18289 18267 18325 18293</t>
+  </si>
+  <si>
+    <t>BubbleSort 512000 73329 73112 73291 73244</t>
+  </si>
+  <si>
+    <t>BubbleSort 1000000 280605 280184 279859 280216</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 1000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 2000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 4000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 8000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 16000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 32000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 64000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 128000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 256000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 512000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 1000000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Insertion Sort 1000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Insertion Sort 2000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Insertion Sort 4000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Insertion Sort 8000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Insertion Sort 16000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Insertion Sort 32000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Insertion Sort 64000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Insertion Sort 128000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Insertion Sort 256000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Insertion Sort 512000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Insertion Sort 1000000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Selection Sort 1000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Selection Sort 2000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Selection Sort 4000 3 3 3 3</t>
+  </si>
+  <si>
+    <t>Selection Sort 8000 15 15 15 15</t>
+  </si>
+  <si>
+    <t>Selection Sort 16000 60 60 60 60</t>
+  </si>
+  <si>
+    <t>Selection Sort 32000 260 240 240 246</t>
+  </si>
+  <si>
+    <t>Selection Sort 64000 974 960 963 965</t>
+  </si>
+  <si>
+    <t>Selection Sort 128000 3865 3867 3845 3859</t>
+  </si>
+  <si>
+    <t>Selection Sort 256000 15412 15432 15504 15449</t>
+  </si>
+  <si>
+    <t>Selection Sort 512000 62295 62211 62070 62192</t>
+  </si>
+  <si>
+    <t>Selection Sort 1000000 237881 237484 237421 237595</t>
+  </si>
+  <si>
+    <t>Heap Sort 1000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Heap Sort 2000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Heap Sort 4000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Heap Sort 8000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Heap Sort 16000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Heap Sort 32000 1 1 1 1</t>
+  </si>
+  <si>
+    <t>Heap Sort 64000 2 2 2 2</t>
+  </si>
+  <si>
+    <t>Heap Sort 128000 5 5 5 5</t>
+  </si>
+  <si>
+    <t>Heap Sort 256000 11 11 11 11</t>
+  </si>
+  <si>
+    <t>Heap Sort 512000 25 25 25 25</t>
+  </si>
+  <si>
+    <t>Heap Sort 1000000 53 53 53 53</t>
+  </si>
+  <si>
+    <t>Merge Sort 1000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Merge Sort 2000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Merge Sort 4000 1 1 1 1</t>
+  </si>
+  <si>
+    <t>Merge Sort 8000 2 2 2 2</t>
+  </si>
+  <si>
+    <t>Merge Sort 16000 5 5 5 5</t>
+  </si>
+  <si>
+    <t>Merge Sort 32000 10 10 13 11</t>
+  </si>
+  <si>
+    <t>Merge Sort 64000 21 21 21 21</t>
+  </si>
+  <si>
+    <t>Merge Sort 128000 43 44 44 43</t>
+  </si>
+  <si>
+    <t>Merge Sort 256000 90 89 88 89</t>
+  </si>
+  <si>
+    <t>Merge Sort 512000 182 180 179 180</t>
+  </si>
+  <si>
+    <t>Merge Sort 1000000 373 360 360 364</t>
+  </si>
+  <si>
+    <t>Quick Sort 1000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Quick Sort 2000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Quick Sort 4000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Quick Sort 8000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Quick Sort 16000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Quick Sort 32000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Quick Sort 64000 1 1 1 1</t>
+  </si>
+  <si>
+    <t>Quick Sort 128000 2 2 2 2</t>
+  </si>
+  <si>
+    <t>Quick Sort 256000 5 6 5 5</t>
+  </si>
+  <si>
+    <t>Quick Sort 512000 11 11 11 11</t>
+  </si>
+  <si>
+    <t>Quick Sort 1000000 22 22 22 22</t>
+  </si>
+  <si>
+    <t>Radix Sort 1000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Radix Sort 2000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Radix Sort 4000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Radix Sort 8000 1 1 1 1</t>
+  </si>
+  <si>
+    <t>Radix Sort 16000 3 3 3 3</t>
+  </si>
+  <si>
+    <t>Radix Sort 32000 6 6 6 6</t>
+  </si>
+  <si>
+    <t>Radix Sort 64000 11 11 11 11</t>
+  </si>
+  <si>
+    <t>Radix Sort 128000 24 23 24 23</t>
+  </si>
+  <si>
+    <t>Radix Sort 256000 50 50 49 49</t>
+  </si>
+  <si>
+    <t>Radix Sort 512000 102 101 101 101</t>
+  </si>
+  <si>
+    <t>Radix Sort 1000000 197 197 209 201</t>
+  </si>
+  <si>
+    <t>Counting Sort 1000 7 6 6 6</t>
+  </si>
+  <si>
+    <t>Counting Sort 2000 7 7 6 6</t>
+  </si>
+  <si>
+    <t>Counting Sort 4000 6 6 7 6</t>
+  </si>
+  <si>
+    <t>Counting Sort 8000 7 7 7 7</t>
+  </si>
+  <si>
+    <t>Counting Sort 16000 7 7 7 7</t>
+  </si>
+  <si>
+    <t>Counting Sort 32000 7 7 7 7</t>
+  </si>
+  <si>
+    <t>Counting Sort 64000 8 7 7 7</t>
+  </si>
+  <si>
+    <t>Counting Sort 128000 8 7 9 8</t>
+  </si>
+  <si>
+    <t>Counting Sort 256000 9 8 8 8</t>
+  </si>
+  <si>
+    <t>Counting Sort 512000 10 11 11 10</t>
+  </si>
+  <si>
+    <t>Counting Sort 1000000 14 14 14 14</t>
+  </si>
+  <si>
+    <t>Smooth Sort 1000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Smooth Sort 2000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Smooth Sort 4000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Smooth Sort 8000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Smooth Sort 16000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Smooth Sort 32000 0 0 0 0</t>
+  </si>
+  <si>
+    <t>Smooth Sort 64000 1 1 1 1</t>
+  </si>
+  <si>
+    <t>Smooth Sort 128000 2 2 2 2</t>
+  </si>
+  <si>
+    <t>Smooth Sort 256000 5 4 5 4</t>
+  </si>
+  <si>
+    <t>Smooth Sort 512000 9 10 13 10</t>
+  </si>
+  <si>
+    <t>Smooth Sort 1000000 20 20 21 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Descending</t>
+  </si>
+  <si>
+    <t>BubbleSort 1000 1 1 1 1</t>
+  </si>
+  <si>
+    <t>BubbleSort 2000 6 5 5 5</t>
+  </si>
+  <si>
+    <t>BubbleSort 4000 25 25 25 25</t>
+  </si>
+  <si>
+    <t>BubbleSort 8000 104 104 110 106</t>
+  </si>
+  <si>
+    <t>BubbleSort 16000 429 428 426 427</t>
+  </si>
+  <si>
+    <t>BubbleSort 32000 1708 1704 1710 1707</t>
+  </si>
+  <si>
+    <t>BubbleSort 64000 6819 6829 6813 6820</t>
+  </si>
+  <si>
+    <t>BubbleSort 128000 27225 27250 27246 27240</t>
+  </si>
+  <si>
+    <t>BubbleSort 256000 108839 108816 108772 108809</t>
+  </si>
+  <si>
+    <t>BubbleSort 512000 435332 434458 434248 434679</t>
+  </si>
+  <si>
+    <t>BubbleSort 1000000 1655293 1655707 1655780 1655593</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 2000 1 1 1 1</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 4000 9 10 10 9</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 8000 67 68 68 67</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 16000 346 345 345 345</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 32000 1546 1544 1549 1546</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 64000 6520 6520 6517 6519</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 128000 26606 26540 26556 26567</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 256000 106815 106805 106780 106800</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 512000 428411 427874 427690 427991</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 1000000 1632317 1631902 1632468 1632229</t>
+  </si>
+  <si>
+    <t>Insertion Sort 2000 1 1 1 1</t>
+  </si>
+  <si>
+    <t>Insertion Sort 4000 7 7 7 7</t>
+  </si>
+  <si>
+    <t>Insertion Sort 8000 31 31 31 31</t>
+  </si>
+  <si>
+    <t>Insertion Sort 16000 128 130 128 128</t>
+  </si>
+  <si>
+    <t>Insertion Sort 32000 515 517 518 516</t>
+  </si>
+  <si>
+    <t>Insertion Sort 64000 2067 2069 2068 2068</t>
+  </si>
+  <si>
+    <t>Insertion Sort 128000 8297 8299 8300 8298</t>
+  </si>
+  <si>
+    <t>Insertion Sort 256000 33217 33181 33229 33209</t>
+  </si>
+  <si>
+    <t>Insertion Sort 512000 132965 132943 132761 132889</t>
+  </si>
+  <si>
+    <t>Insertion Sort 1000000 507286 507087 507191 507188</t>
+  </si>
+  <si>
+    <t>Selection Sort 2000 1 1 1 1</t>
+  </si>
+  <si>
+    <t>Selection Sort 4000 7 7 7 7</t>
+  </si>
+  <si>
+    <t>Selection Sort 8000 40 40 40 40</t>
+  </si>
+  <si>
+    <t>Selection Sort 16000 191 191 192 191</t>
+  </si>
+  <si>
+    <t>Selection Sort 32000 820 818 818 818</t>
+  </si>
+  <si>
+    <t>Selection Sort 64000 3411 3402 3409 3407</t>
+  </si>
+  <si>
+    <t>Selection Sort 128000 13810 13818 13826 13818</t>
+  </si>
+  <si>
+    <t>Selection Sort 256000 55377 55419 55361 55385</t>
+  </si>
+  <si>
+    <t>Selection Sort 512000 222517 222217 222250 222328</t>
+  </si>
+  <si>
+    <t>Selection Sort 1000000 847833 847944 847989 847922</t>
+  </si>
+  <si>
+    <t>Heap Sort 256000 12 11 11 11</t>
+  </si>
+  <si>
+    <t>Heap Sort 512000 24 25 24 24</t>
+  </si>
+  <si>
+    <t>Heap Sort 1000000 51 51 52 51</t>
+  </si>
+  <si>
+    <t>Merge Sort 32000 10 10 10 10</t>
+  </si>
+  <si>
+    <t>Merge Sort 64000 22 21 21 21</t>
+  </si>
+  <si>
+    <t>Merge Sort 256000 89 89 91 89</t>
+  </si>
+  <si>
+    <t>Merge Sort 512000 183 182 182 182</t>
+  </si>
+  <si>
+    <t>Merge Sort 1000000 368 366 371 368</t>
+  </si>
+  <si>
+    <t>Quick Sort 256000 5 5 5 5</t>
+  </si>
+  <si>
+    <t>Quick Sort 512000 12 12 12 12</t>
+  </si>
+  <si>
+    <t>Quick Sort 1000000 24 24 24 24</t>
+  </si>
+  <si>
+    <t>Radix Sort 64000 12 12 12 12</t>
+  </si>
+  <si>
+    <t>Radix Sort 128000 25 25 25 25</t>
+  </si>
+  <si>
+    <t>Radix Sort 256000 51 51 51 51</t>
+  </si>
+  <si>
+    <t>Radix Sort 512000 102 102 100 101</t>
+  </si>
+  <si>
+    <t>Radix Sort 1000000 194 192 194 193</t>
+  </si>
+  <si>
+    <t>Counting Sort 2000 6 6 6 6</t>
+  </si>
+  <si>
+    <t>Counting Sort 4000 6 6 6 6</t>
+  </si>
+  <si>
+    <t>Counting Sort 8000 6 6 6 6</t>
+  </si>
+  <si>
+    <t>Counting Sort 16000 6 6 7 6</t>
+  </si>
+  <si>
+    <t>Counting Sort 64000 7 7 7 7</t>
+  </si>
+  <si>
+    <t>Counting Sort 128000 7 7 7 7</t>
+  </si>
+  <si>
+    <t>Counting Sort 256000 8 9 9 8</t>
+  </si>
+  <si>
+    <t>Counting Sort 512000 11 10 10 10</t>
+  </si>
+  <si>
+    <t>Smooth Sort 16000 1 1 1 1</t>
+  </si>
+  <si>
+    <t>Smooth Sort 32000 2 2 2 2</t>
+  </si>
+  <si>
+    <t>Smooth Sort 64000 6 6 6 6</t>
+  </si>
+  <si>
+    <t>Smooth Sort 128000 12 12 13 12</t>
+  </si>
+  <si>
+    <t>Smooth Sort 256000 25 25 25 25</t>
+  </si>
+  <si>
+    <t>Smooth Sort 512000 52 56 52 53</t>
+  </si>
+  <si>
+    <t>Smooth Sort 1000000 105 105 106 105</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Random</t>
+  </si>
+  <si>
+    <t>BubbleSort 2000 4 4 4 4</t>
+  </si>
+  <si>
+    <t>BubbleSort 4000 19 19 19 19</t>
+  </si>
+  <si>
+    <t>BubbleSort 8000 79 79 80 79</t>
+  </si>
+  <si>
+    <t>BubbleSort 16000 324 325 322 323</t>
+  </si>
+  <si>
+    <t>BubbleSort 32000 1301 1296 1298 1298</t>
+  </si>
+  <si>
+    <t>BubbleSort 64000 5272 5280 5274 5275</t>
+  </si>
+  <si>
+    <t>BubbleSort 128000 21182 21230 21192 21201</t>
+  </si>
+  <si>
+    <t>BubbleSort 256000 86748 86710 86670 86709</t>
+  </si>
+  <si>
+    <t>BubbleSort 512000 355449 355543 355545 355512</t>
+  </si>
+  <si>
+    <t>BubbleSort 1000000 1373564 1373897 1373741 1373734</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 2000 2 2 2 2</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 4000 10 10 10 10</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 8000 57 57 59 57</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 16000 276 277 275 276</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 32000 1230 1226 1227 1227</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 64000 5168 5161 5152 5160</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 128000 20985 20976 20972 20977</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 256000 85605 85526 85615 85582</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 512000 351347 351399 351573 351439</t>
+  </si>
+  <si>
+    <t>BubbleSort with Flag 1000000 1357454 1357522 1357972 1357649</t>
+  </si>
+  <si>
+    <t>Insertion Sort 4000 4 3 3 3</t>
+  </si>
+  <si>
+    <t>Insertion Sort 8000 15 15 15 15</t>
+  </si>
+  <si>
+    <t>Insertion Sort 16000 64 63 63 63</t>
+  </si>
+  <si>
+    <t>Insertion Sort 32000 258 256 255 256</t>
+  </si>
+  <si>
+    <t>Insertion Sort 64000 1034 1037 1039 1036</t>
+  </si>
+  <si>
+    <t>Insertion Sort 128000 4149 4156 4140 4148</t>
+  </si>
+  <si>
+    <t>Insertion Sort 256000 16604 16633 16596 16611</t>
+  </si>
+  <si>
+    <t>Insertion Sort 512000 66567 66596 66505 66556</t>
+  </si>
+  <si>
+    <t>Insertion Sort 1000000 253653 253785 253591 253676</t>
+  </si>
+  <si>
+    <t>Selection Sort 16000 62 61 61 61</t>
+  </si>
+  <si>
+    <t>Selection Sort 32000 244 241 241 242</t>
+  </si>
+  <si>
+    <t>Selection Sort 64000 963 965 963 963</t>
+  </si>
+  <si>
+    <t>Selection Sort 128000 3867 3870 3864 3867</t>
+  </si>
+  <si>
+    <t>Selection Sort 256000 15440 15415 15437 15430</t>
+  </si>
+  <si>
+    <t>Selection Sort 512000 61858 61678 61844 61793</t>
+  </si>
+  <si>
+    <t>Selection Sort 1000000 235785 235811 235938 235844</t>
+  </si>
+  <si>
+    <t>Heap Sort 64000 3 3 3 3</t>
+  </si>
+  <si>
+    <t>Heap Sort 128000 7 7 7 7</t>
+  </si>
+  <si>
+    <t>Heap Sort 256000 17 18 18 17</t>
+  </si>
+  <si>
+    <t>Heap Sort 512000 45 45 45 45</t>
+  </si>
+  <si>
+    <t>Heap Sort 1000000 105 103 105 104</t>
+  </si>
+  <si>
+    <t>Merge Sort 32000 12 12 12 12</t>
+  </si>
+  <si>
+    <t>Merge Sort 64000 25 24 25 24</t>
+  </si>
+  <si>
+    <t>Merge Sort 128000 53 50 50 51</t>
+  </si>
+  <si>
+    <t>Merge Sort 256000 104 104 103 103</t>
+  </si>
+  <si>
+    <t>Merge Sort 512000 213 213 211 212</t>
+  </si>
+  <si>
+    <t>Merge Sort 1000000 430 429 429 429</t>
+  </si>
+  <si>
+    <t>Quick Sort 32000 1 1 1 1</t>
+  </si>
+  <si>
+    <t>Quick Sort 64000 3 3 3 3</t>
+  </si>
+  <si>
+    <t>Quick Sort 128000 7 7 8 7</t>
+  </si>
+  <si>
+    <t>Quick Sort 256000 16 16 16 16</t>
+  </si>
+  <si>
+    <t>Quick Sort 512000 35 35 35 35</t>
+  </si>
+  <si>
+    <t>Quick Sort 1000000 72 71 72 71</t>
+  </si>
+  <si>
+    <t>Radix Sort 16000 2 2 2 2</t>
+  </si>
+  <si>
+    <t>Radix Sort 32000 5 5 5 5</t>
+  </si>
+  <si>
+    <t>Radix Sort 128000 23 23 23 23</t>
+  </si>
+  <si>
+    <t>Radix Sort 256000 47 47 47 47</t>
+  </si>
+  <si>
+    <t>Radix Sort 512000 96 97 95 96</t>
+  </si>
+  <si>
+    <t>Radix Sort 1000000 194 196 197 195</t>
+  </si>
+  <si>
+    <t>Counting Sort 1000 7 7 6 6</t>
+  </si>
+  <si>
+    <t>Counting Sort 16000 7 6 6 6</t>
+  </si>
+  <si>
+    <t>Counting Sort 128000 8 8 8 8</t>
+  </si>
+  <si>
+    <t>Counting Sort 256000 9 9 9 9</t>
+  </si>
+  <si>
+    <t>Counting Sort 512000 13 12 12 12</t>
+  </si>
+  <si>
+    <t>Counting Sort 1000000 16 15 15 15</t>
+  </si>
+  <si>
+    <t>Smooth Sort 8000 0 1 0 0</t>
+  </si>
+  <si>
+    <t>Smooth Sort 16000 2 2 2 2</t>
+  </si>
+  <si>
+    <t>Smooth Sort 32000 4 4 4 4</t>
+  </si>
+  <si>
+    <t>Smooth Sort 64000 9 9 9 9</t>
+  </si>
+  <si>
+    <t>Smooth Sort 128000 21 22 20 21</t>
+  </si>
+  <si>
+    <t>Smooth Sort 256000 45 48 45 46</t>
+  </si>
+  <si>
+    <t>Smooth Sort 512000 105 100 100 101</t>
+  </si>
+  <si>
+    <t>Smooth Sort 1000000 212 212 212 212</t>
   </si>
 </sst>
 </file>
@@ -96,7 +885,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -104,13 +893,120 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -299,28 +1195,28 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>280</c:v>
+                  <c:v>285</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1126</c:v>
+                  <c:v>1133</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4520</c:v>
+                  <c:v>4536</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18121</c:v>
+                  <c:v>18293</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>72340</c:v>
+                  <c:v>73244</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>276881</c:v>
+                  <c:v>280216</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -689,25 +1585,25 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>240</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>963</c:v>
+                  <c:v>965</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3848</c:v>
+                  <c:v>3859</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15397</c:v>
+                  <c:v>15449</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>61676</c:v>
+                  <c:v>62192</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>235894</c:v>
+                  <c:v>237595</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -833,7 +1729,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>53</c:v>
@@ -950,7 +1846,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>21</c:v>
@@ -962,10 +1858,10 @@
                   <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>179</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>360</c:v>
+                  <c:v>364</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1094,13 +1990,13 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1217,25 +2113,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>91</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>175</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1349,28 +2245,28 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1493,19 +2389,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1882,37 +2778,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69</c:v>
+                  <c:v>427</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>280</c:v>
+                  <c:v>1707</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1126</c:v>
+                  <c:v>6820</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4520</c:v>
+                  <c:v>27240</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18121</c:v>
+                  <c:v>108809</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>72340</c:v>
+                  <c:v>494679</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>276881</c:v>
+                  <c:v>1655593</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2014,34 +2910,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>345</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1546</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>6519</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>26567</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>106800</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>427991</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1632229</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2143,34 +3039,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>516</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2068</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>8298</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>33209</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>132889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>507188</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2272,34 +3168,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63</c:v>
+                  <c:v>191</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>240</c:v>
+                  <c:v>818</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>963</c:v>
+                  <c:v>3407</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3848</c:v>
+                  <c:v>13818</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15397</c:v>
+                  <c:v>55385</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>61676</c:v>
+                  <c:v>222328</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>235894</c:v>
+                  <c:v>847922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2425,10 +3321,10 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>53</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2554,10 +3450,10 @@
                   <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>179</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>360</c:v>
+                  <c:v>368</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2686,13 +3582,13 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2809,25 +3705,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>91</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>175</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2950,19 +3846,19 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3079,25 +3975,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3474,37 +4370,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69</c:v>
+                  <c:v>323</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>280</c:v>
+                  <c:v>1298</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1126</c:v>
+                  <c:v>5275</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4520</c:v>
+                  <c:v>21201</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18121</c:v>
+                  <c:v>86709</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>72340</c:v>
+                  <c:v>355512</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>276881</c:v>
+                  <c:v>1373734</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3606,34 +4502,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1227</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>5160</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>20977</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>85582</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>351439</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1357649</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3735,34 +4631,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1036</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>4148</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1661</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>66556</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>253676</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3864,7 +4760,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -3873,25 +4769,25 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>240</c:v>
+                  <c:v>242</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>963</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3848</c:v>
+                  <c:v>3867</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15397</c:v>
+                  <c:v>15430</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>61676</c:v>
+                  <c:v>61793</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>235894</c:v>
+                  <c:v>235844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4008,19 +4904,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>53</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4134,22 +5030,22 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>179</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>360</c:v>
+                  <c:v>429</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4269,22 +5165,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4407,19 +5303,19 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>91</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>175</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4542,19 +5438,19 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4671,25 +5567,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6953,13 +7849,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668F2229-9767-4B25-B4EC-86A2DA35ED88}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -7103,7 +8002,7 @@
         <v>8000</v>
       </c>
       <c r="B5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -7127,7 +8026,7 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -7147,7 +8046,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -7159,10 +8058,10 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -7173,7 +8072,7 @@
         <v>32000</v>
       </c>
       <c r="B7">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -7182,19 +8081,19 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J7">
         <v>7</v>
@@ -7208,7 +8107,7 @@
         <v>64000</v>
       </c>
       <c r="B8">
-        <v>1126</v>
+        <v>1133</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -7217,7 +8116,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -7229,13 +8128,13 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -7243,7 +8142,7 @@
         <v>128000</v>
       </c>
       <c r="B9">
-        <v>4520</v>
+        <v>4536</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -7252,7 +8151,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>3848</v>
+        <v>3859</v>
       </c>
       <c r="F9">
         <v>5</v>
@@ -7264,13 +8163,13 @@
         <v>2</v>
       </c>
       <c r="I9">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -7278,7 +8177,7 @@
         <v>256000</v>
       </c>
       <c r="B10">
-        <v>18121</v>
+        <v>18293</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -7287,7 +8186,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>15397</v>
+        <v>15449</v>
       </c>
       <c r="F10">
         <v>11</v>
@@ -7296,16 +8195,16 @@
         <v>89</v>
       </c>
       <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>49</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
         <v>4</v>
-      </c>
-      <c r="I10">
-        <v>45</v>
-      </c>
-      <c r="J10">
-        <v>7</v>
-      </c>
-      <c r="K10">
-        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -7313,7 +8212,7 @@
         <v>512000</v>
       </c>
       <c r="B11">
-        <v>72340</v>
+        <v>73244</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -7322,25 +8221,25 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>61676</v>
+        <v>62192</v>
       </c>
       <c r="F11">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G11">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H11">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I11">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="J11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K11">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -7348,7 +8247,7 @@
         <v>1000000</v>
       </c>
       <c r="B12">
-        <v>276881</v>
+        <v>280216</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -7357,25 +8256,25 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>235894</v>
+        <v>237595</v>
       </c>
       <c r="F12">
         <v>53</v>
       </c>
       <c r="G12">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="H12">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I12">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="J12">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K12">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -7383,7 +8282,122 @@
         <v>10</v>
       </c>
     </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="10"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B18:J27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -7392,10 +8406,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15AC7A6F-609C-4464-9EBA-177C314D7C55}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="B18" sqref="B18:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7437,7 +8451,7 @@
         <v>1000</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -7472,16 +8486,16 @@
         <v>2000</v>
       </c>
       <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7507,16 +8521,16 @@
         <v>4000</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -7542,16 +8556,16 @@
         <v>8000</v>
       </c>
       <c r="B5">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -7577,16 +8591,16 @@
         <v>16000</v>
       </c>
       <c r="B6">
-        <v>69</v>
+        <v>427</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>345</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="E6">
-        <v>63</v>
+        <v>191</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -7598,13 +8612,13 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6">
         <v>6</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -7612,16 +8626,16 @@
         <v>32000</v>
       </c>
       <c r="B7">
-        <v>280</v>
+        <v>1707</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1546</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>516</v>
       </c>
       <c r="E7">
-        <v>240</v>
+        <v>818</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -7633,13 +8647,13 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J7">
         <v>7</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -7647,16 +8661,16 @@
         <v>64000</v>
       </c>
       <c r="B8">
-        <v>1126</v>
+        <v>6820</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>6519</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2068</v>
       </c>
       <c r="E8">
-        <v>963</v>
+        <v>3407</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -7668,13 +8682,13 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
         <v>6</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -7682,16 +8696,16 @@
         <v>128000</v>
       </c>
       <c r="B9">
-        <v>4520</v>
+        <v>27240</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>26567</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>8298</v>
       </c>
       <c r="E9">
-        <v>3848</v>
+        <v>13818</v>
       </c>
       <c r="F9">
         <v>5</v>
@@ -7703,13 +8717,13 @@
         <v>2</v>
       </c>
       <c r="I9">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J9">
         <v>7</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -7717,16 +8731,16 @@
         <v>256000</v>
       </c>
       <c r="B10">
-        <v>18121</v>
+        <v>108809</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>106800</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>33209</v>
       </c>
       <c r="E10">
-        <v>15397</v>
+        <v>55385</v>
       </c>
       <c r="F10">
         <v>11</v>
@@ -7735,16 +8749,16 @@
         <v>89</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I10">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="J10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -7752,34 +8766,34 @@
         <v>512000</v>
       </c>
       <c r="B11">
-        <v>72340</v>
+        <v>494679</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>427991</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>132889</v>
       </c>
       <c r="E11">
-        <v>61676</v>
+        <v>222328</v>
       </c>
       <c r="F11">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G11">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H11">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I11">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="J11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K11">
-        <v>5</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -7787,34 +8801,34 @@
         <v>1000000</v>
       </c>
       <c r="B12">
-        <v>276881</v>
+        <v>1655593</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1632229</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>507188</v>
       </c>
       <c r="E12">
-        <v>235894</v>
+        <v>847922</v>
       </c>
       <c r="F12">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G12">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="H12">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I12">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="J12">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K12">
-        <v>10</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -7822,7 +8836,122 @@
         <v>10</v>
       </c>
     </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="10"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B18:J27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -7830,10 +8959,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1968C521-4591-489E-94A3-553A12659E33}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="B18" sqref="B18:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7875,7 +9004,7 @@
         <v>1000</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -7910,16 +9039,16 @@
         <v>2000</v>
       </c>
       <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7945,13 +9074,13 @@
         <v>4000</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -7980,13 +9109,13 @@
         <v>8000</v>
       </c>
       <c r="B5">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -8015,16 +9144,16 @@
         <v>16000</v>
       </c>
       <c r="B6">
-        <v>69</v>
+        <v>323</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>276</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="E6">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -8042,7 +9171,7 @@
         <v>6</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -8050,25 +9179,25 @@
         <v>32000</v>
       </c>
       <c r="B7">
-        <v>280</v>
+        <v>1298</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1227</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="E7">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>5</v>
@@ -8077,7 +9206,7 @@
         <v>7</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -8085,34 +9214,34 @@
         <v>64000</v>
       </c>
       <c r="B8">
-        <v>1126</v>
+        <v>5275</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>5160</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1036</v>
       </c>
       <c r="E8">
         <v>963</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -8120,34 +9249,34 @@
         <v>128000</v>
       </c>
       <c r="B9">
-        <v>4520</v>
+        <v>21201</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>20977</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>4148</v>
       </c>
       <c r="E9">
-        <v>3848</v>
+        <v>3867</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G9">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I9">
+        <v>23</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
         <v>21</v>
-      </c>
-      <c r="J9">
-        <v>7</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -8155,34 +9284,34 @@
         <v>256000</v>
       </c>
       <c r="B10">
-        <v>18121</v>
+        <v>86709</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>85582</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1661</v>
       </c>
       <c r="E10">
-        <v>15397</v>
+        <v>15430</v>
       </c>
       <c r="F10">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G10">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I10">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J10">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -8190,34 +9319,34 @@
         <v>512000</v>
       </c>
       <c r="B11">
-        <v>72340</v>
+        <v>355512</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>351439</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>66556</v>
       </c>
       <c r="E11">
-        <v>61676</v>
+        <v>61793</v>
       </c>
       <c r="F11">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="G11">
-        <v>179</v>
+        <v>212</v>
       </c>
       <c r="H11">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="I11">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="J11">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K11">
-        <v>5</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -8225,34 +9354,34 @@
         <v>1000000</v>
       </c>
       <c r="B12">
-        <v>276881</v>
+        <v>1373734</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1357649</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>253676</v>
       </c>
       <c r="E12">
-        <v>235894</v>
+        <v>235844</v>
       </c>
       <c r="F12">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="G12">
-        <v>360</v>
+        <v>429</v>
       </c>
       <c r="H12">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="I12">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="J12">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K12">
-        <v>10</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -8260,8 +9389,1834 @@
         <v>10</v>
       </c>
     </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B18:J27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{322C49A0-A0D5-4B97-AB98-23244A0960D7}">
+  <dimension ref="A1:A339"/>
+  <sheetViews>
+    <sheetView topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>271</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>